<commit_message>
부동산뱅크 DB반영 ERD 부동산뱅크 과거시세 MIG simpleBatchContext 추가(main 함수 실행용) setSoup2TableDic > TableDic 추가(text 기본형) fetch Exception 보강 insertBasicByTBLDicList ListInsert Crawling 객체 반영 Telegram SendMessage 보강(4096 제한으로 쪼개서 송신)
</commit_message>
<xml_diff>
--- a/51.Dev/Column2REP_TABLE.xlsx
+++ b/51.Dev/Column2REP_TABLE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="11600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="11600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="컬럼리스트" sheetId="1" r:id="rId1"/>
@@ -27,133 +27,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
-  <si>
-    <t>dealCount</t>
-  </si>
-  <si>
-    <t>leaseCount</t>
-  </si>
-  <si>
-    <t>rentCount</t>
-  </si>
-  <si>
-    <t>shortTermRentCount</t>
-  </si>
-  <si>
-    <t>dealPriceMin</t>
-  </si>
-  <si>
-    <t>dealPriceMax</t>
-  </si>
-  <si>
-    <t>dealPricePerSpaceMin</t>
-  </si>
-  <si>
-    <t>dealPricePerSpaceMax</t>
-  </si>
-  <si>
-    <t>dealPriceString</t>
-  </si>
-  <si>
-    <t>dealPricePerSpaceString</t>
-  </si>
-  <si>
-    <t>leasePriceString</t>
-  </si>
-  <si>
-    <t>leasePricePerSpaceString</t>
-  </si>
-  <si>
-    <t>leasePriceRateString</t>
-  </si>
-  <si>
-    <t>SALE_CNT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+  <si>
+    <t>BB_CMPX_ID</t>
+  </si>
+  <si>
+    <t>REG_USER_ID</t>
+  </si>
+  <si>
+    <t>REG_DTM</t>
+  </si>
+  <si>
+    <t>CHG_USER_ID</t>
+  </si>
+  <si>
+    <t>CHG_DTM</t>
+  </si>
+  <si>
+    <t>BB_CMPX_TYP_SEQ</t>
+  </si>
+  <si>
+    <t>STD_YYMM</t>
+  </si>
+  <si>
+    <t>STD_YMD</t>
+  </si>
+  <si>
+    <t>DOWN_PRC</t>
+  </si>
+  <si>
+    <t>UP_PRC</t>
+  </si>
+  <si>
+    <t>CHG_PRC</t>
+  </si>
+  <si>
+    <t>DOWN_JS_PRC</t>
+  </si>
+  <si>
+    <t>UP_JS_PRC</t>
+  </si>
+  <si>
+    <t>CHG_JS_PRC</t>
+  </si>
+  <si>
+    <t>sdate_ym</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JS_CNT</t>
+    <t>sdate_ymd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WS_CNT</t>
+    <t>prc_l</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SHRT_RENT_CNT</t>
+    <t>prc_h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MSML_PRC_AMT_STR</t>
+    <t>change_prc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MBIG_PRC_AMT_STR</t>
+    <t>rnt_l</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MSML_PYNG_PER_AMT</t>
+    <t>rnt_h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MBIG_PYNG_PER_AMT</t>
+    <t>change_굿</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMT_STR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PYNG_PER_AMT_STR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JS_PRC_STR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JS_PYNG_PER_PRC_STR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JS_PRC_RATE_STR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JOB_ID</t>
-  </si>
-  <si>
-    <t>JOB_SEQ</t>
-  </si>
-  <si>
-    <t>EXEC_PERD_CD</t>
-  </si>
-  <si>
-    <t>EXEC_MM</t>
-  </si>
-  <si>
-    <t>EXEC_DD</t>
-  </si>
-  <si>
-    <t>EXEC_HH</t>
-  </si>
-  <si>
-    <t>EXEC_MI</t>
-  </si>
-  <si>
-    <t>EXEC_DAY_CD</t>
-  </si>
-  <si>
-    <t>CYCL_MI</t>
-  </si>
-  <si>
-    <t>IMDI_EXEC_YN</t>
-  </si>
-  <si>
-    <t>USE_YN</t>
-  </si>
-  <si>
-    <t>DEL_YN</t>
   </si>
 </sst>
 </file>
@@ -486,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A1:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -499,62 +446,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -567,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -579,462 +536,462 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="str">
         <f>CONCATENATE("'",컬럼리스트!A1,"' : None,")</f>
-        <v>'JOB_ID' : None,</v>
+        <v>'BB_CMPX_ID' : None,</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>CONCATENATE("'",컬럼리스트!A2,"' : None,")</f>
-        <v>'JOB_SEQ' : None,</v>
+        <v>'BB_CMPX_TYP_SEQ' : None,</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>CONCATENATE("'",컬럼리스트!A3,"' : None,")</f>
-        <v>'EXEC_PERD_CD' : None,</v>
+        <v>'STD_YYMM' : None,</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>CONCATENATE("'",컬럼리스트!A4,"' : None,")</f>
-        <v>'EXEC_MM' : None,</v>
+        <v>'STD_YMD' : None,</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>CONCATENATE("'",컬럼리스트!A5,"' : None,")</f>
-        <v>'EXEC_DD' : None,</v>
+        <v>'DOWN_PRC' : None,</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f>CONCATENATE("'",컬럼리스트!A6,"' : None,")</f>
-        <v>'EXEC_HH' : None,</v>
+        <v>'UP_PRC' : None,</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>CONCATENATE("'",컬럼리스트!A7,"' : None,")</f>
-        <v>'EXEC_MI' : None,</v>
+        <v>'CHG_PRC' : None,</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>CONCATENATE("'",컬럼리스트!A8,"' : None,")</f>
-        <v>'EXEC_DAY_CD' : None,</v>
+        <v>'DOWN_JS_PRC' : None,</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f>CONCATENATE("'",컬럼리스트!A9,"' : None,")</f>
-        <v>'CYCL_MI' : None,</v>
+        <v>'UP_JS_PRC' : None,</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>CONCATENATE("'",컬럼리스트!A10,"' : None,")</f>
-        <v>'IMDI_EXEC_YN' : None,</v>
+        <v>'CHG_JS_PRC' : None,</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f>CONCATENATE("'",컬럼리스트!A11,"' : None,")</f>
-        <v>'USE_YN' : None,</v>
+        <v>'REG_USER_ID' : None,</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f>CONCATENATE("'",컬럼리스트!A12,"' : None,")</f>
-        <v>'DEL_YN' : None,</v>
+        <v>'REG_DTM' : None,</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A13" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A13,"' : None,")</f>
+        <v>'CHG_USER_ID' : None,</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A14" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A14,"' : None,")</f>
+        <v>'CHG_DTM' : None,</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A15" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A15,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A16" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A16,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A17" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A17,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A18" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A18,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A19" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A19,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A20" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A20,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="e">
-        <f>CONCATENATE("'",컬럼리스트!#REF!,"' : None,")</f>
-        <v>#REF!</v>
+      <c r="A21" t="str">
+        <f>CONCATENATE("'",컬럼리스트!A21,"' : None,")</f>
+        <v>'' : None,</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A13,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A22,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A14,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A23,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A15,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A24,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A16,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A25,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A17,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A26,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A18,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A27,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A19,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A28,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A20,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A29,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A21,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A30,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A22,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A31,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A23,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A32,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A24,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A33,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A25,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A34,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A26,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A35,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A27,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A36,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A28,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A37,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A29,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A38,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A30,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A39,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A31,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A40,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A32,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A41,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A33,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A42,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A34,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A43,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A35,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A44,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A36,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A45,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A37,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A46,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A38,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A47,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A39,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A48,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A40,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A49,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A41,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A50,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A42,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A51,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A43,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A52,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A44,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A53,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A45,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A54,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A46,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A55,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A47,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A56,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A48,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A57,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A49,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A58,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A50,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A59,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A51,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A60,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A52,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A61,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A53,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A62,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A54,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A63,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A55,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A64,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A56,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A65,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A57,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A66,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A58,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A67,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A59,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A68,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A60,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A69,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A61,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A70,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A62,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A71,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A63,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A72,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A64,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A73,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A65,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A74,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A66,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A75,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A67,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A76,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" t="str">
-        <f>CONCATENATE("'",컬럼리스트!A68,"' : None,")</f>
+        <f>CONCATENATE("'",컬럼리스트!A77,"' : None,")</f>
         <v>'' : None,</v>
       </c>
     </row>
@@ -1047,119 +1004,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1173,93 +1121,96 @@
   <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="str">
-        <f>CONCATENATE("'",Mapping리스트!A1,"' : '",Mapping리스트!B1,"',")</f>
-        <v>'dealCount' : 'SALE_CNT',</v>
+        <f>CONCATENATE("'",Mapping리스트!A3,"' : '",Mapping리스트!B1,"',")</f>
+        <v>'sdate_ym' : 'BB_CMPX_ID',</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>CONCATENATE("'",Mapping리스트!A2,"' : '",Mapping리스트!B2,"',")</f>
-        <v>'leaseCount' : 'JS_CNT',</v>
+        <v>'' : 'BB_CMPX_TYP_SEQ',</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="str">
-        <f>CONCATENATE("'",Mapping리스트!A3,"' : '",Mapping리스트!B3,"',")</f>
-        <v>'rentCount' : 'WS_CNT',</v>
+      <c r="A3" t="e">
+        <f>CONCATENATE("'",Mapping리스트!#REF!,"' : '",Mapping리스트!B3,"',")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>CONCATENATE("'",Mapping리스트!A4,"' : '",Mapping리스트!B4,"',")</f>
-        <v>'shortTermRentCount' : 'SHRT_RENT_CNT',</v>
+        <v>'sdate_ymd' : 'STD_YMD',</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>CONCATENATE("'",Mapping리스트!A5,"' : '",Mapping리스트!B5,"',")</f>
-        <v>'dealPriceMin' : 'MSML_PRC_AMT_STR',</v>
+        <v>'prc_l' : 'DOWN_PRC',</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f>CONCATENATE("'",Mapping리스트!A6,"' : '",Mapping리스트!B6,"',")</f>
-        <v>'dealPriceMax' : 'MBIG_PRC_AMT_STR',</v>
+        <v>'prc_h' : 'UP_PRC',</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>CONCATENATE("'",Mapping리스트!A7,"' : '",Mapping리스트!B7,"',")</f>
-        <v>'dealPricePerSpaceMin' : 'MSML_PYNG_PER_AMT',</v>
+        <v>'change_prc' : 'CHG_PRC',</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>CONCATENATE("'",Mapping리스트!A8,"' : '",Mapping리스트!B8,"',")</f>
-        <v>'dealPricePerSpaceMax' : 'MBIG_PYNG_PER_AMT',</v>
+        <v>'rnt_l' : 'DOWN_JS_PRC',</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f>CONCATENATE("'",Mapping리스트!A9,"' : '",Mapping리스트!B9,"',")</f>
-        <v>'dealPriceString' : 'AMT_STR',</v>
+        <v>'rnt_h' : 'UP_JS_PRC',</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>CONCATENATE("'",Mapping리스트!A10,"' : '",Mapping리스트!B10,"',")</f>
-        <v>'dealPricePerSpaceString' : 'PYNG_PER_AMT_STR',</v>
+        <v>'change_굿' : 'CHG_JS_PRC',</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f>CONCATENATE("'",Mapping리스트!A11,"' : '",Mapping리스트!B11,"',")</f>
-        <v>'leasePriceString' : 'JS_PRC_STR',</v>
+        <v>'' : 'REG_USER_ID',</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f>CONCATENATE("'",Mapping리스트!A12,"' : '",Mapping리스트!B12,"',")</f>
-        <v>'leasePricePerSpaceString' : 'JS_PYNG_PER_PRC_STR',</v>
+        <v>'' : 'REG_DTM',</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f>CONCATENATE("'",Mapping리스트!A13,"' : '",Mapping리스트!B13,"',")</f>
-        <v>'leasePriceRateString' : 'JS_PRC_RATE_STR',</v>
+        <v>'' : 'CHG_USER_ID',</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>CONCATENATE("'",Mapping리스트!A14,"' : '",Mapping리스트!B14,"',")</f>
-        <v>'' : '',</v>
+        <v>'' : 'CHG_DTM',</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">

</xml_diff>